<commit_message>
Fixed the change of direction
Now you can change direction without glitches
The width and the height of each level are stores in the first 2 bytes of datamap.bin
</commit_message>
<xml_diff>
--- a/mytest.xlsx
+++ b/mytest.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SDCC\MSX_Fusion-C_V1.3\WorkingFolder\fusion-c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE43345F-69A9-4AAD-AA65-93341AC83B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF363AA8-01A7-4BC5-A42B-F2BF25D4287F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26175" yWindow="1110" windowWidth="21600" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="right to left" sheetId="2" r:id="rId2"/>
     <sheet name="left to right" sheetId="3" r:id="rId3"/>
+    <sheet name="confronto" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>S</t>
   </si>
@@ -52,12 +53,46 @@
   <si>
     <t>NX</t>
   </si>
+  <si>
+    <t>last col sorg</t>
+  </si>
+  <si>
+    <t>last col dest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="_-* #,##0.00000000000\ _€_-;\-* #,##0.00000000000\ _€_-;_-* &quot;-&quot;???????????\ _€_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0.0000000000000000000_-;\-* #,##0.0000000000000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,8 +156,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -145,11 +192,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -161,8 +368,47 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,19 +687,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:JQ26"/>
+  <dimension ref="A1:JQ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="IG1" sqref="IG1:IU1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="IO31" sqref="IO31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="2.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="28" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="27" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="100" width="3.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="101" max="230" width="4.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="231" max="256" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="101" max="222" width="4.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="223" max="224" width="4.140625" style="1" customWidth="1"/>
+    <col min="225" max="225" width="4.140625" style="13" customWidth="1"/>
+    <col min="226" max="230" width="4.140625" style="1" customWidth="1"/>
+    <col min="231" max="244" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="3.42578125" style="1" customWidth="1"/>
+    <col min="246" max="256" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="257" max="257" width="4" bestFit="1" customWidth="1"/>
     <col min="265" max="265" width="4" bestFit="1" customWidth="1"/>
     <col min="269" max="269" width="4" bestFit="1" customWidth="1"/>
@@ -1135,7 +1387,7 @@
       <c r="HP1" s="1">
         <v>223</v>
       </c>
-      <c r="HQ1" s="1">
+      <c r="HQ1" s="13">
         <v>224</v>
       </c>
       <c r="HR1" s="1">
@@ -1457,7 +1709,7 @@
       <c r="HN2" s="2"/>
       <c r="HO2" s="2"/>
       <c r="HP2" s="2"/>
-      <c r="HQ2" s="2"/>
+      <c r="HQ2" s="14"/>
       <c r="HR2" s="2"/>
       <c r="HS2" s="2"/>
       <c r="HT2" s="2"/>
@@ -1706,7 +1958,7 @@
       <c r="HN3" s="3"/>
       <c r="HO3" s="3"/>
       <c r="HP3" s="3"/>
-      <c r="HQ3" s="3"/>
+      <c r="HQ3" s="15"/>
       <c r="HR3" s="3"/>
       <c r="HS3" s="3"/>
       <c r="HT3" s="3"/>
@@ -1947,7 +2199,7 @@
       <c r="HN4" s="4"/>
       <c r="HO4" s="4"/>
       <c r="HP4" s="4"/>
-      <c r="HQ4" s="4"/>
+      <c r="HQ4" s="16"/>
       <c r="HR4" s="4"/>
       <c r="HS4" s="4"/>
       <c r="HT4" s="4"/>
@@ -2192,7 +2444,7 @@
       <c r="HN5" s="5"/>
       <c r="HO5" s="5"/>
       <c r="HP5" s="5"/>
-      <c r="HQ5" s="5"/>
+      <c r="HQ5" s="17"/>
       <c r="HR5" s="5"/>
       <c r="HS5" s="5"/>
       <c r="HT5" s="5"/>
@@ -2437,7 +2689,7 @@
       <c r="HN6" s="6"/>
       <c r="HO6" s="6"/>
       <c r="HP6" s="6"/>
-      <c r="HQ6" s="6"/>
+      <c r="HQ6" s="18"/>
       <c r="HR6" s="6"/>
       <c r="HS6" s="6"/>
       <c r="HT6" s="6"/>
@@ -2678,7 +2930,7 @@
       <c r="HN7" s="7"/>
       <c r="HO7" s="7"/>
       <c r="HP7" s="7"/>
-      <c r="HQ7" s="7"/>
+      <c r="HQ7" s="19"/>
       <c r="HR7" s="7"/>
       <c r="HS7" s="7"/>
       <c r="HT7" s="7"/>
@@ -2919,7 +3171,7 @@
       <c r="HN8" s="8"/>
       <c r="HO8" s="8"/>
       <c r="HP8" s="8"/>
-      <c r="HQ8" s="8"/>
+      <c r="HQ8" s="20"/>
       <c r="HR8" s="8"/>
       <c r="HS8" s="8"/>
       <c r="HT8" s="8"/>
@@ -3160,7 +3412,7 @@
       <c r="HN9" s="9"/>
       <c r="HO9" s="9"/>
       <c r="HP9" s="9"/>
-      <c r="HQ9" s="9"/>
+      <c r="HQ9" s="21"/>
       <c r="HR9" s="9"/>
       <c r="HS9" s="9"/>
       <c r="HT9" s="9"/>
@@ -3401,7 +3653,7 @@
       <c r="HN10" s="2"/>
       <c r="HO10" s="2"/>
       <c r="HP10" s="2"/>
-      <c r="HQ10" s="2"/>
+      <c r="HQ10" s="14"/>
       <c r="HR10" s="2"/>
       <c r="HS10" s="2"/>
       <c r="HT10" s="2"/>
@@ -3642,7 +3894,7 @@
       <c r="HN11" s="3"/>
       <c r="HO11" s="3"/>
       <c r="HP11" s="3"/>
-      <c r="HQ11" s="3"/>
+      <c r="HQ11" s="15"/>
       <c r="HR11" s="3"/>
       <c r="HS11" s="3"/>
       <c r="HT11" s="3"/>
@@ -3889,7 +4141,7 @@
       <c r="HN12" s="4"/>
       <c r="HO12" s="4"/>
       <c r="HP12" s="4"/>
-      <c r="HQ12" s="4"/>
+      <c r="HQ12" s="16"/>
       <c r="HR12" s="4"/>
       <c r="HS12" s="4"/>
       <c r="HT12" s="4"/>
@@ -4150,7 +4402,7 @@
       <c r="HN13" s="5"/>
       <c r="HO13" s="5"/>
       <c r="HP13" s="5"/>
-      <c r="HQ13" s="5"/>
+      <c r="HQ13" s="17"/>
       <c r="HR13" s="5"/>
       <c r="HS13" s="5"/>
       <c r="HT13" s="5"/>
@@ -4410,7 +4662,7 @@
       <c r="HN14" s="6"/>
       <c r="HO14" s="6"/>
       <c r="HP14" s="6"/>
-      <c r="HQ14" s="6"/>
+      <c r="HQ14" s="18"/>
       <c r="HR14" s="6"/>
       <c r="HS14" s="6"/>
       <c r="HT14" s="6"/>
@@ -4442,19 +4694,19 @@
         <v>13</v>
       </c>
       <c r="JM14">
-        <f t="shared" ref="JM14:JM26" si="0">JM13-16</f>
+        <f t="shared" ref="JM14:JM24" si="0">JM13-16</f>
         <v>192</v>
       </c>
       <c r="JN14">
-        <f t="shared" ref="JN14:JN26" si="1">JM14+15</f>
+        <f t="shared" ref="JN14:JN24" si="1">JM14+15</f>
         <v>207</v>
       </c>
       <c r="JP14">
-        <f t="shared" ref="JP14:JP26" si="2">JP13-16</f>
+        <f t="shared" ref="JP14:JP24" si="2">JP13-16</f>
         <v>208</v>
       </c>
       <c r="JQ14">
-        <f t="shared" ref="JQ14:JQ26" si="3">JP14+15</f>
+        <f t="shared" ref="JQ14:JQ24" si="3">JP14+15</f>
         <v>223</v>
       </c>
     </row>
@@ -4670,7 +4922,7 @@
       <c r="HN15" s="7"/>
       <c r="HO15" s="7"/>
       <c r="HP15" s="7"/>
-      <c r="HQ15" s="7"/>
+      <c r="HQ15" s="19"/>
       <c r="HR15" s="7"/>
       <c r="HS15" s="7"/>
       <c r="HT15" s="7"/>
@@ -4930,7 +5182,7 @@
       <c r="HN16" s="8"/>
       <c r="HO16" s="8"/>
       <c r="HP16" s="8"/>
-      <c r="HQ16" s="8"/>
+      <c r="HQ16" s="20"/>
       <c r="HR16" s="8"/>
       <c r="HS16" s="8"/>
       <c r="HT16" s="8"/>
@@ -4980,7 +5232,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:277" x14ac:dyDescent="0.25">
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
@@ -5190,7 +5442,7 @@
       <c r="HN17" s="9"/>
       <c r="HO17" s="9"/>
       <c r="HP17" s="9"/>
-      <c r="HQ17" s="9"/>
+      <c r="HQ17" s="21"/>
       <c r="HR17" s="9"/>
       <c r="HS17" s="9"/>
       <c r="HT17" s="9"/>
@@ -5241,7 +5493,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:277" x14ac:dyDescent="0.25">
       <c r="JI18">
         <v>9</v>
       </c>
@@ -5262,7 +5514,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:277" x14ac:dyDescent="0.25">
       <c r="IP19" s="1">
         <f>240+15-1</f>
         <v>254</v>
@@ -5291,7 +5543,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:277" x14ac:dyDescent="0.25">
       <c r="JI20">
         <v>7</v>
       </c>
@@ -5312,7 +5564,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:277" x14ac:dyDescent="0.25">
       <c r="IP21" s="1">
         <f>224</f>
         <v>224</v>
@@ -5344,7 +5596,53 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:277" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24">
+        <v>0</v>
+      </c>
+      <c r="C22" s="24">
+        <v>1</v>
+      </c>
+      <c r="D22" s="24">
+        <v>2</v>
+      </c>
+      <c r="E22" s="24">
+        <v>3</v>
+      </c>
+      <c r="F22" s="24">
+        <v>4</v>
+      </c>
+      <c r="G22" s="24">
+        <v>5</v>
+      </c>
+      <c r="H22" s="24">
+        <v>6</v>
+      </c>
+      <c r="I22" s="24">
+        <v>7</v>
+      </c>
+      <c r="J22" s="24">
+        <v>8</v>
+      </c>
+      <c r="K22" s="24">
+        <v>9</v>
+      </c>
+      <c r="L22" s="24">
+        <v>10</v>
+      </c>
+      <c r="M22" s="24">
+        <v>11</v>
+      </c>
+      <c r="N22" s="24">
+        <v>12</v>
+      </c>
+      <c r="O22" s="24">
+        <v>13</v>
+      </c>
+      <c r="P22" s="24">
+        <v>14</v>
+      </c>
       <c r="JI22">
         <v>5</v>
       </c>
@@ -5365,1202 +5663,726 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="16:277" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="23"/>
       <c r="JI23">
+        <v>2</v>
+      </c>
+      <c r="JM23" t="e">
+        <f>#REF!-16</f>
+        <v>#REF!</v>
+      </c>
+      <c r="JN23" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="JP23" t="e">
+        <f>#REF!-16</f>
+        <v>#REF!</v>
+      </c>
+      <c r="JQ23" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A24" s="30"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="23"/>
+      <c r="JI24">
+        <v>1</v>
+      </c>
+      <c r="JM24" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="JN24" t="e">
+        <f t="shared" si="1"/>
+        <v>#REF!</v>
+      </c>
+      <c r="JP24" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="JQ24" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:277" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="23"/>
+    </row>
+    <row r="26" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="26"/>
+    </row>
+    <row r="27" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+    </row>
+    <row r="28" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+    </row>
+    <row r="29" spans="1:277" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="24">
+        <v>1</v>
+      </c>
+      <c r="B29" s="24">
+        <v>2</v>
+      </c>
+      <c r="C29" s="24">
+        <v>3</v>
+      </c>
+      <c r="D29" s="24">
         <v>4</v>
       </c>
-      <c r="JM23">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="JN23">
-        <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="JP23">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
-      <c r="JQ23">
-        <f t="shared" si="3"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="16:277" x14ac:dyDescent="0.25">
-      <c r="JI24">
-        <v>3</v>
-      </c>
-      <c r="JM24">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="JN24">
-        <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="JP24">
-        <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-      <c r="JQ24">
-        <f t="shared" si="3"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="16:277" x14ac:dyDescent="0.25">
-      <c r="JI25">
-        <v>2</v>
-      </c>
-      <c r="JM25">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="JN25">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="JP25">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="JQ25">
-        <f t="shared" si="3"/>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="16:277" x14ac:dyDescent="0.25">
-      <c r="JI26">
-        <v>1</v>
-      </c>
-      <c r="JM26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="JN26">
-        <f t="shared" si="1"/>
+      <c r="E29" s="24">
+        <v>5</v>
+      </c>
+      <c r="F29" s="24">
+        <v>6</v>
+      </c>
+      <c r="G29" s="24">
+        <v>7</v>
+      </c>
+      <c r="H29" s="24">
+        <v>8</v>
+      </c>
+      <c r="I29" s="24">
+        <v>9</v>
+      </c>
+      <c r="J29" s="24">
+        <v>10</v>
+      </c>
+      <c r="K29" s="24">
+        <v>11</v>
+      </c>
+      <c r="L29" s="24">
+        <v>12</v>
+      </c>
+      <c r="M29" s="24">
+        <v>13</v>
+      </c>
+      <c r="N29" s="24">
+        <v>14</v>
+      </c>
+      <c r="O29" s="1">
         <v>15</v>
       </c>
-      <c r="JP26">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="JQ26">
-        <f t="shared" si="3"/>
-        <v>31</v>
-      </c>
+    </row>
+    <row r="30" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="23"/>
+    </row>
+    <row r="31" spans="1:277" x14ac:dyDescent="0.25">
+      <c r="A31" s="40"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="23"/>
+    </row>
+    <row r="32" spans="1:277" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="42"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="23"/>
+    </row>
+    <row r="33" spans="1:245" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="23"/>
+      <c r="IK33" s="48"/>
+    </row>
+    <row r="34" spans="1:245" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="23"/>
+    </row>
+    <row r="35" spans="1:245" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="32"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="23"/>
+    </row>
+    <row r="36" spans="1:245" x14ac:dyDescent="0.25">
+      <c r="IK36" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D99220-F6CC-4BFB-AC1E-93FA5C6873E6}">
-  <dimension ref="C1:O64"/>
+  <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="K1" t="str">
-        <f>DEC2HEX(I1,2)</f>
-        <v>00</v>
-      </c>
-      <c r="M1">
-        <f>I1+64</f>
+    <row r="1" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <f>16*B3</f>
+        <v>224</v>
+      </c>
+      <c r="F3">
+        <f>E3+16</f>
+        <v>240</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <f>E3+H3-1</f>
+        <v>239</v>
+      </c>
+      <c r="K3">
+        <f>F3+H3-1</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E16" si="0">16*B4</f>
+        <v>208</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F16" si="1">E4+16</f>
+        <v>224</v>
+      </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J17" si="2">E4+H4-1</f>
+        <v>223</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K17" si="3">F4+H4-1</f>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>207</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="H10">
+        <v>16</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="H12">
+        <v>16</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="O1" t="str">
-        <f>DEC2HEX(M1,2)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="str">
-        <f t="shared" ref="K2:K64" si="0">DEC2HEX(I2,2)</f>
-        <v>01</v>
-      </c>
-      <c r="M2">
-        <f t="shared" ref="M2:M64" si="1">I2+64</f>
-        <v>65</v>
-      </c>
-      <c r="O2" t="str">
-        <f t="shared" ref="O2:O64" si="2">DEC2HEX(M2,2)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I3">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>16</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="H14">
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="K3" t="str">
+      <c r="E15">
         <f t="shared" si="0"/>
-        <v>02</v>
-      </c>
-      <c r="M3">
+        <v>32</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="O3" t="str">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="K4" t="str">
-        <f t="shared" si="0"/>
-        <v>03</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" si="2"/>
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>240</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="0"/>
-        <v>04</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="2"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <f>14*16</f>
-        <v>224</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="0"/>
-        <v>05</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <f>C5-C6</f>
-        <v>16</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="0"/>
-        <v>06</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="2"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="0"/>
-        <v>07</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="O8" t="str">
+        <v>48</v>
+      </c>
+      <c r="H15">
+        <v>16</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="K9" t="str">
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="0"/>
-        <v>08</v>
-      </c>
-      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="O9" t="str">
+        <v>32</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="2"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I10">
-        <v>9</v>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="0"/>
-        <v>09</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="O10" t="str">
+        <v>31</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="2"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="K11" t="str">
-        <f t="shared" si="0"/>
-        <v>0A</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="2"/>
-        <v>4A</v>
-      </c>
-    </row>
-    <row r="12" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I12">
-        <v>11</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="0"/>
-        <v>0B</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="2"/>
-        <v>4B</v>
-      </c>
-    </row>
-    <row r="13" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I13">
-        <v>12</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v>0C</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="1"/>
-        <v>76</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="2"/>
-        <v>4C</v>
-      </c>
-    </row>
-    <row r="14" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I14">
-        <v>13</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="0"/>
-        <v>0D</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="2"/>
-        <v>4D</v>
-      </c>
-    </row>
-    <row r="15" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I15">
-        <v>14</v>
-      </c>
-      <c r="K15" t="str">
-        <f t="shared" si="0"/>
-        <v>0E</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="2"/>
-        <v>4E</v>
-      </c>
-    </row>
-    <row r="16" spans="3:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I16">
         <v>15</v>
       </c>
-      <c r="K16" t="str">
-        <f t="shared" si="0"/>
-        <v>0F</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="2"/>
-        <v>4F</v>
-      </c>
-    </row>
-    <row r="17" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I17">
-        <v>16</v>
-      </c>
-      <c r="K17" t="str">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I18">
-        <v>17</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I19">
-        <v>18</v>
-      </c>
-      <c r="K19" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" si="2"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I20">
-        <v>19</v>
-      </c>
-      <c r="K20" t="str">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" si="2"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I21">
-        <v>20</v>
-      </c>
-      <c r="K21" t="str">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" si="2"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I22">
-        <v>21</v>
-      </c>
-      <c r="K22" t="str">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" si="2"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I23">
-        <v>22</v>
-      </c>
-      <c r="K23" t="str">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I24">
-        <v>23</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I25">
-        <v>24</v>
-      </c>
-      <c r="K25" t="str">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" si="2"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I26">
-        <v>25</v>
-      </c>
-      <c r="K26" t="str">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I27">
-        <v>26</v>
-      </c>
-      <c r="K27" t="str">
-        <f t="shared" si="0"/>
-        <v>1A</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="O27" t="str">
-        <f t="shared" si="2"/>
-        <v>5A</v>
-      </c>
-    </row>
-    <row r="28" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I28">
-        <v>27</v>
-      </c>
-      <c r="K28" t="str">
-        <f t="shared" si="0"/>
-        <v>1B</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="O28" t="str">
-        <f t="shared" si="2"/>
-        <v>5B</v>
-      </c>
-    </row>
-    <row r="29" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I29">
-        <v>28</v>
-      </c>
-      <c r="K29" t="str">
-        <f t="shared" si="0"/>
-        <v>1C</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="O29" t="str">
-        <f t="shared" si="2"/>
-        <v>5C</v>
-      </c>
-    </row>
-    <row r="30" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I30">
-        <v>29</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="0"/>
-        <v>1D</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="O30" t="str">
-        <f t="shared" si="2"/>
-        <v>5D</v>
-      </c>
-    </row>
-    <row r="31" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I31">
-        <v>30</v>
-      </c>
-      <c r="K31" t="str">
-        <f t="shared" si="0"/>
-        <v>1E</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="O31" t="str">
-        <f t="shared" si="2"/>
-        <v>5E</v>
-      </c>
-    </row>
-    <row r="32" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I32">
+      <c r="K17">
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="K32" t="str">
-        <f t="shared" si="0"/>
-        <v>1F</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="O32" t="str">
-        <f t="shared" si="2"/>
-        <v>5F</v>
-      </c>
-    </row>
-    <row r="33" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I33">
-        <v>32</v>
-      </c>
-      <c r="K33" t="str">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="O33" t="str">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I34">
-        <v>33</v>
-      </c>
-      <c r="K34" t="str">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="O34" t="str">
-        <f t="shared" si="2"/>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I35">
-        <v>34</v>
-      </c>
-      <c r="K35" t="str">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="O35" t="str">
-        <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I36">
-        <v>35</v>
-      </c>
-      <c r="K36" t="str">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="O36" t="str">
-        <f t="shared" si="2"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I37">
-        <v>36</v>
-      </c>
-      <c r="K37" t="str">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="O37" t="str">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I38">
-        <v>37</v>
-      </c>
-      <c r="K38" t="str">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="O38" t="str">
-        <f t="shared" si="2"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I39">
-        <v>38</v>
-      </c>
-      <c r="K39" t="str">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="O39" t="str">
-        <f t="shared" si="2"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I40">
-        <v>39</v>
-      </c>
-      <c r="K40" t="str">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="M40">
-        <f t="shared" si="1"/>
-        <v>103</v>
-      </c>
-      <c r="O40" t="str">
-        <f t="shared" si="2"/>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I41">
-        <v>40</v>
-      </c>
-      <c r="K41" t="str">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="O41" t="str">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I42">
-        <v>41</v>
-      </c>
-      <c r="K42" t="str">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="M42">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="O42" t="str">
-        <f t="shared" si="2"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I43">
-        <v>42</v>
-      </c>
-      <c r="K43" t="str">
-        <f t="shared" si="0"/>
-        <v>2A</v>
-      </c>
-      <c r="M43">
-        <f t="shared" si="1"/>
-        <v>106</v>
-      </c>
-      <c r="O43" t="str">
-        <f t="shared" si="2"/>
-        <v>6A</v>
-      </c>
-    </row>
-    <row r="44" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I44">
-        <v>43</v>
-      </c>
-      <c r="K44" t="str">
-        <f t="shared" si="0"/>
-        <v>2B</v>
-      </c>
-      <c r="M44">
-        <f t="shared" si="1"/>
-        <v>107</v>
-      </c>
-      <c r="O44" t="str">
-        <f t="shared" si="2"/>
-        <v>6B</v>
-      </c>
-    </row>
-    <row r="45" spans="9:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="I45">
-        <v>44</v>
-      </c>
-      <c r="K45" t="str">
-        <f t="shared" si="0"/>
-        <v>2C</v>
-      </c>
-      <c r="M45">
-        <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="O45" t="str">
-        <f t="shared" si="2"/>
-        <v>6C</v>
-      </c>
-    </row>
-    <row r="46" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I46">
-        <v>45</v>
-      </c>
-      <c r="K46" t="str">
-        <f t="shared" si="0"/>
-        <v>2D</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="O46" t="str">
-        <f t="shared" si="2"/>
-        <v>6D</v>
-      </c>
-    </row>
-    <row r="47" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I47">
-        <v>46</v>
-      </c>
-      <c r="K47" t="str">
-        <f t="shared" si="0"/>
-        <v>2E</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-      <c r="O47" t="str">
-        <f t="shared" si="2"/>
-        <v>6E</v>
-      </c>
-    </row>
-    <row r="48" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I48">
-        <v>47</v>
-      </c>
-      <c r="K48" t="str">
-        <f t="shared" si="0"/>
-        <v>2F</v>
-      </c>
-      <c r="M48">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="O48" t="str">
-        <f t="shared" si="2"/>
-        <v>6F</v>
-      </c>
-    </row>
-    <row r="49" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I49">
-        <v>48</v>
-      </c>
-      <c r="K49" t="str">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="M49">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-      <c r="O49" t="str">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I50">
-        <v>49</v>
-      </c>
-      <c r="K50" t="str">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="M50">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="O50" t="str">
-        <f t="shared" si="2"/>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I51">
-        <v>50</v>
-      </c>
-      <c r="K51" t="str">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="M51">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="O51" t="str">
-        <f t="shared" si="2"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I52">
-        <v>51</v>
-      </c>
-      <c r="K52" t="str">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-      <c r="O52" t="str">
-        <f t="shared" si="2"/>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I53">
-        <v>52</v>
-      </c>
-      <c r="K53" t="str">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="M53">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="O53" t="str">
-        <f t="shared" si="2"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I54">
-        <v>53</v>
-      </c>
-      <c r="K54" t="str">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="M54">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="O54" t="str">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I55">
-        <v>54</v>
-      </c>
-      <c r="K55" t="str">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="M55">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="O55" t="str">
-        <f t="shared" si="2"/>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I56">
-        <v>55</v>
-      </c>
-      <c r="K56" t="str">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="O56" t="str">
-        <f t="shared" si="2"/>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I57">
-        <v>56</v>
-      </c>
-      <c r="K57" t="str">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-      <c r="O57" t="str">
-        <f t="shared" si="2"/>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I58">
-        <v>57</v>
-      </c>
-      <c r="K58" t="str">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="M58">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-      <c r="O58" t="str">
-        <f t="shared" si="2"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="59" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I59">
-        <v>58</v>
-      </c>
-      <c r="K59" t="str">
-        <f t="shared" si="0"/>
-        <v>3A</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="1"/>
-        <v>122</v>
-      </c>
-      <c r="O59" t="str">
-        <f t="shared" si="2"/>
-        <v>7A</v>
-      </c>
-    </row>
-    <row r="60" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I60">
-        <v>59</v>
-      </c>
-      <c r="K60" t="str">
-        <f t="shared" si="0"/>
-        <v>3B</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-      <c r="O60" t="str">
-        <f t="shared" si="2"/>
-        <v>7B</v>
-      </c>
-    </row>
-    <row r="61" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I61">
-        <v>60</v>
-      </c>
-      <c r="K61" t="str">
-        <f t="shared" si="0"/>
-        <v>3C</v>
-      </c>
-      <c r="M61">
-        <f t="shared" si="1"/>
-        <v>124</v>
-      </c>
-      <c r="O61" t="str">
-        <f t="shared" si="2"/>
-        <v>7C</v>
-      </c>
-    </row>
-    <row r="62" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I62">
-        <v>61</v>
-      </c>
-      <c r="K62" t="str">
-        <f t="shared" si="0"/>
-        <v>3D</v>
-      </c>
-      <c r="M62">
-        <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-      <c r="O62" t="str">
-        <f t="shared" si="2"/>
-        <v>7D</v>
-      </c>
-    </row>
-    <row r="63" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I63">
-        <v>62</v>
-      </c>
-      <c r="K63" t="str">
-        <f t="shared" si="0"/>
-        <v>3E</v>
-      </c>
-      <c r="M63">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="O63" t="str">
-        <f t="shared" si="2"/>
-        <v>7E</v>
-      </c>
-    </row>
-    <row r="64" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I64">
-        <v>63</v>
-      </c>
-      <c r="K64" t="str">
-        <f t="shared" si="0"/>
-        <v>3F</v>
-      </c>
-      <c r="M64">
-        <f t="shared" si="1"/>
-        <v>127</v>
-      </c>
-      <c r="O64" t="str">
-        <f t="shared" si="2"/>
-        <v>7F</v>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f>SUM(H3:H17)</f>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -6570,33 +6392,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C7DC3E8-7C44-4DF6-A40B-236162FA7A51}">
-  <dimension ref="B1:K17"/>
+  <dimension ref="B1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
+    <row r="1" spans="2:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="12" t="s">
         <v>4</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -6955,6 +6787,740 @@
       <c r="K17">
         <f t="shared" si="2"/>
         <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f>SUM(H3:H17)</f>
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B2ED0F-E372-4B24-A338-036E9E4F7580}">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H15" si="0">H3+16</f>
+        <v>240</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I16" si="1">H2-16</f>
+        <v>224</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="N2">
+        <v>15</v>
+      </c>
+      <c r="O2">
+        <v>16</v>
+      </c>
+      <c r="P2">
+        <f>O2-16</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B16" si="2">16*A3</f>
+        <v>224</v>
+      </c>
+      <c r="C3">
+        <f>B3+16</f>
+        <v>240</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="2"/>
+        <v>208</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C16" si="3">B4+16</f>
+        <v>224</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="K4">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>13</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O16" si="4">O5+16</f>
+        <v>240</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P17" si="5">O4-16</f>
+        <v>224</v>
+      </c>
+      <c r="R4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
+      <c r="E5">
+        <v>16</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="K5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>224</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="5"/>
+        <v>208</v>
+      </c>
+      <c r="R5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="3"/>
+        <v>192</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+      <c r="N6">
+        <v>11</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="4"/>
+        <v>208</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="R6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>176</v>
+      </c>
+      <c r="E7">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="K7">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>10</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>192</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="5"/>
+        <v>176</v>
+      </c>
+      <c r="R7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>160</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="K8">
+        <v>16</v>
+      </c>
+      <c r="N8">
+        <v>9</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+      <c r="R8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+      <c r="R9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="K10">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="R10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="5"/>
+        <v>112</v>
+      </c>
+      <c r="R11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="K12">
+        <v>16</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
+      <c r="R12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="K13">
+        <v>16</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="R13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K14">
+        <v>16</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="R14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="K15">
+        <v>16</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="R15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>16</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="R16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>O2+16</f>
+        <v>32</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="R17">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>